<commit_message>
Added: Try catch error handling.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corma\Documents\#Development\VS22\SquirrelEngine-CMP316\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalWorkDir\2200592\SquirrelEngine-CMP316\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{480E7AD1-40F2-4310-9AA4-CD9F65896FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1F0B17-A817-429E-AF5A-941304DEC550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10296" yWindow="1968" windowWidth="20760" windowHeight="12204" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Error Codes</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>Failed to create rasterizer state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entry </t>
+  </si>
+  <si>
+    <t>Options File failed to open</t>
+  </si>
+  <si>
+    <t>Options file has no window name</t>
+  </si>
+  <si>
+    <t>Options file has no window size</t>
+  </si>
+  <si>
+    <t>Options file window size formatted incorrectly</t>
+  </si>
+  <si>
+    <t>Options file has no on load nut</t>
+  </si>
+  <si>
+    <t>main</t>
   </si>
 </sst>
 </file>
@@ -464,17 +485,17 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -488,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -502,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -516,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -530,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -544,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -558,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -572,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
@@ -586,7 +607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
@@ -600,7 +621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
@@ -614,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -628,62 +649,77 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14</v>
       </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added: Error codes to sheet
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalWorkDir\2200592\SquirrelEngine-CMP316\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1F0B17-A817-429E-AF5A-941304DEC550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD1BF2A-4F40-4322-A3D1-E7D8B0B63070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>Error Codes</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>main</t>
+  </si>
+  <si>
+    <t>Shelled Nut being loaded but a nut inside it has no type</t>
+  </si>
+  <si>
+    <t>ShelledNut</t>
+  </si>
+  <si>
+    <t>Instantiate</t>
+  </si>
+  <si>
+    <t>Nut</t>
+  </si>
+  <si>
+    <t>Deserialize</t>
   </si>
 </sst>
 </file>
@@ -482,16 +497,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8609D8BE-0152-4021-92E2-EC9D22BAD52D}">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -723,11 +738,28 @@
       <c r="B18">
         <v>16</v>
       </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: Error codes 18 & 19 to doc
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalWorkDir\2200592\SquirrelEngine-CMP316\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalWorkDir\2200592\SquirrelEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD1BF2A-4F40-4322-A3D1-E7D8B0B63070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9579C645-5E25-455D-8AAF-A29C347A1B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Error Codes</t>
   </si>
@@ -120,6 +120,24 @@
   </si>
   <si>
     <t>Deserialize</t>
+  </si>
+  <si>
+    <t>Mesh</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Error Loading Mesh</t>
+  </si>
+  <si>
+    <t>Pool Allocation Service Unknown Error</t>
+  </si>
+  <si>
+    <t>PoolAllocationService</t>
+  </si>
+  <si>
+    <t>MakeUniquePoolPtr</t>
   </si>
 </sst>
 </file>
@@ -497,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8609D8BE-0152-4021-92E2-EC9D22BAD52D}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,6 +780,34 @@
         <v>27</v>
       </c>
     </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: Player Set target/limit FPS
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corma\Documents\#Development\VS22\SquirrelEngine-CMP316\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACA7277-26C8-42C9-A63D-44E3239B9EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D2436-3CCE-447A-B105-0F126CA33405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="2100" windowWidth="20760" windowHeight="12204" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
+    <workbookView xWindow="816" yWindow="456" windowWidth="20760" windowHeight="12204" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Error Codes</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t xml:space="preserve">Trying to allocate to a full pool. </t>
+  </si>
+  <si>
+    <t>Background colour not set</t>
+  </si>
+  <si>
+    <t>Background colour wrong format</t>
+  </si>
+  <si>
+    <t>Target FPS not set</t>
   </si>
 </sst>
 </file>
@@ -524,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8609D8BE-0152-4021-92E2-EC9D22BAD52D}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,13 +831,55 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>34</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: Tidy and polish
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corma\Documents\#Development\VS22\SquirrelEngine-CMP316\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889D6CC8-4950-4D16-98FF-E158D8A78B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A396FB-0A02-479A-960E-50A13F9638CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="816" yWindow="456" windowWidth="20760" windowHeight="12204" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Error Codes</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>Pool block size too small or blocks not aligned. Make block size more than or equal to 8, and divisible by 8.</t>
+  </si>
+  <si>
+    <t>Physics Nut does not have a collision shape when ready called</t>
+  </si>
+  <si>
+    <t>PhysicsNut</t>
+  </si>
+  <si>
+    <t>Ready</t>
   </si>
 </sst>
 </file>
@@ -536,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8609D8BE-0152-4021-92E2-EC9D22BAD52D}">
-  <dimension ref="B2:E26"/>
+  <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
@@ -899,6 +908,20 @@
         <v>34</v>
       </c>
     </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: Documentation & Report
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corma\Documents\#Development\VS22\SquirrelEngine-CMP316\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A396FB-0A02-479A-960E-50A13F9638CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A73254-B0D0-4A27-B399-97ED859BA9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="816" yWindow="456" windowWidth="20760" windowHeight="12204" xr2:uid="{CA387A30-7C5A-40C5-A7AE-7E485843AE40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>Error Codes</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Ready</t>
+  </si>
+  <si>
+    <t>Shelled Nut being loaded but a nut inside it has no name</t>
   </si>
 </sst>
 </file>
@@ -547,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8609D8BE-0152-4021-92E2-EC9D22BAD52D}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -925,5 +928,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>